<commit_message>
for the pandapower thing, lab1 and lab2 done, lab3 still pending
i just had a tuotira with vinicius
</commit_message>
<xml_diff>
--- a/Lab3 - Timeseries powerflow/results/res_bus/vm_pu.xlsx
+++ b/Lab3 - Timeseries powerflow/results/res_bus/vm_pu.xlsx
@@ -424,34 +424,43 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>1.003961318456261</v>
+        <v>0.991412918452992</v>
       </c>
       <c r="D2">
-        <v>1.006371583623035</v>
+        <v>0.986601626550307</v>
       </c>
       <c r="E2">
-        <v>1.00491661359848</v>
+        <v>0.992613680192833</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G2">
-        <v>1.007308236881191</v>
+        <v>0.974316325861903</v>
       </c>
       <c r="H2">
-        <v>1.007285409982416</v>
+        <v>0.9874975009839858</v>
+      </c>
+      <c r="I2">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J2">
+        <v>0.9868976472291071</v>
+      </c>
+      <c r="K2">
+        <v>0.997709920870801</v>
       </c>
       <c r="L2">
-        <v>1.003927268372521</v>
+        <v>0.991071574230921</v>
       </c>
       <c r="M2">
-        <v>1.006333600792205</v>
+        <v>0.9854014881851936</v>
       </c>
       <c r="N2">
-        <v>1.004882537708171</v>
+        <v>0.9958068879420655</v>
       </c>
       <c r="O2">
-        <v>1.007257981449416</v>
+        <v>0.9706684610392248</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -462,34 +471,43 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>1.003965417594247</v>
+        <v>0.9927068647806099</v>
       </c>
       <c r="D3">
-        <v>1.006379335018004</v>
+        <v>0.9884466247576442</v>
       </c>
       <c r="E3">
-        <v>1.004922100012638</v>
+        <v>0.9938326202608346</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>1.00732202173708</v>
+        <v>0.9771696028160756</v>
       </c>
       <c r="H3">
-        <v>1.007293168415967</v>
+        <v>0.9893441745247911</v>
+      </c>
+      <c r="I3">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J3">
+        <v>0.9887431990110654</v>
+      </c>
+      <c r="K3">
+        <v>0.998983502820711</v>
       </c>
       <c r="L3">
-        <v>1.003931812365842</v>
+        <v>0.992413460816302</v>
       </c>
       <c r="M3">
-        <v>1.006341698207188</v>
+        <v>0.9873358439731758</v>
       </c>
       <c r="N3">
-        <v>1.004888468510511</v>
+        <v>0.9970780406604551</v>
       </c>
       <c r="O3">
-        <v>1.007272804700527</v>
+        <v>0.9738434027420182</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -500,34 +518,43 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1.003953078043938</v>
+        <v>0.9876275637982947</v>
       </c>
       <c r="D4">
-        <v>1.006350794566349</v>
+        <v>0.9806856990150333</v>
       </c>
       <c r="E4">
-        <v>1.004903986321042</v>
+        <v>0.9889005695763177</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>1.007266099891539</v>
+        <v>0.964521919088422</v>
       </c>
       <c r="H4">
-        <v>1.00726460204842</v>
+        <v>0.98157620154572</v>
+      </c>
+      <c r="I4">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J4">
+        <v>0.9809799446745778</v>
+      </c>
+      <c r="K4">
+        <v>0.9940227554399166</v>
       </c>
       <c r="L4">
-        <v>1.003919473154383</v>
+        <v>0.9873324329905674</v>
       </c>
       <c r="M4">
-        <v>1.00631158716339</v>
+        <v>0.9791433665504153</v>
       </c>
       <c r="N4">
-        <v>1.00487035531643</v>
+        <v>0.9921267554143143</v>
       </c>
       <c r="O4">
-        <v>1.007212158259556</v>
+        <v>0.9595980535122357</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -538,34 +565,43 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>1.003953995837598</v>
+        <v>0.9880405230101313</v>
       </c>
       <c r="D5">
-        <v>1.006352913814713</v>
+        <v>0.9813115129876749</v>
       </c>
       <c r="E5">
-        <v>1.004905331338866</v>
+        <v>0.9892982900713927</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="G5">
-        <v>1.007270251015979</v>
+        <v>0.9655416561908783</v>
       </c>
       <c r="H5">
-        <v>1.007266723221148</v>
+        <v>0.9822025837829206</v>
+      </c>
+      <c r="I5">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J5">
+        <v>0.981605946416905</v>
+      </c>
+      <c r="K5">
+        <v>0.9944227909938281</v>
       </c>
       <c r="L5">
-        <v>1.00392039092284</v>
+        <v>0.987745533626158</v>
       </c>
       <c r="M5">
-        <v>1.006313822929723</v>
+        <v>0.9798037843388554</v>
       </c>
       <c r="N5">
-        <v>1.004871700297311</v>
+        <v>0.9925260279399992</v>
       </c>
       <c r="O5">
-        <v>1.007216660919036</v>
+        <v>0.9607499660356039</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -576,34 +612,43 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>1.003930783003759</v>
+        <v>0.9825674952481146</v>
       </c>
       <c r="D6">
-        <v>1.006328251161623</v>
+        <v>0.9759489442219574</v>
       </c>
       <c r="E6">
-        <v>1.004880263699561</v>
+        <v>0.9850001995921686</v>
       </c>
       <c r="F6">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G6">
-        <v>1.007245373945605</v>
+        <v>0.9599594632248213</v>
       </c>
       <c r="H6">
-        <v>1.007242038173365</v>
+        <v>0.9768351455864962</v>
+      </c>
+      <c r="I6">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J6">
+        <v>0.9762417686621047</v>
+      </c>
+      <c r="K6">
+        <v>0.9890080593965691</v>
       </c>
       <c r="L6">
-        <v>1.003889748481143</v>
+        <v>0.9811754057837218</v>
       </c>
       <c r="M6">
-        <v>1.006289150209588</v>
+        <v>0.974422529401186</v>
       </c>
       <c r="N6">
-        <v>1.004839210327368</v>
+        <v>0.9871216244073553</v>
       </c>
       <c r="O6">
-        <v>1.007191751919262</v>
+        <v>0.9550916407657314</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -614,34 +659,43 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1.003943673848713</v>
+        <v>0.991011722163194</v>
       </c>
       <c r="D7">
-        <v>1.006379605514291</v>
+        <v>0.9902495639652201</v>
       </c>
       <c r="E7">
-        <v>1.004905807668983</v>
+        <v>0.9933027343024717</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G7">
-        <v>1.007363394426092</v>
+        <v>0.984741140893128</v>
       </c>
       <c r="H7">
-        <v>1.007293439157875</v>
+        <v>0.9911487508745511</v>
+      </c>
+      <c r="I7">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J7">
+        <v>0.9905466791738494</v>
+      </c>
+      <c r="K7">
+        <v>0.996177732192194</v>
       </c>
       <c r="L7">
-        <v>1.003897020542184</v>
+        <v>0.9884359867814143</v>
       </c>
       <c r="M7">
-        <v>1.006344331855382</v>
+        <v>0.9896517055774779</v>
       </c>
       <c r="N7">
-        <v>1.004859140945008</v>
+        <v>0.9942776217617193</v>
       </c>
       <c r="O7">
-        <v>1.007321226531777</v>
+        <v>0.9831481071063324</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -652,34 +706,43 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>1.003934317529487</v>
+        <v>0.9883965474584619</v>
       </c>
       <c r="D8">
-        <v>1.006365025591068</v>
+        <v>0.9870300066223741</v>
       </c>
       <c r="E8">
-        <v>1.004894485371661</v>
+        <v>0.9909931175490267</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G8">
-        <v>1.007340109875833</v>
+        <v>0.9803816681823642</v>
       </c>
       <c r="H8">
-        <v>1.007278845995488</v>
+        <v>0.9879262700425949</v>
+      </c>
+      <c r="I8">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J8">
+        <v>0.9873261558326467</v>
+      </c>
+      <c r="K8">
+        <v>0.9934294259627219</v>
       </c>
       <c r="L8">
-        <v>1.003886028080455</v>
+        <v>0.9853903811192537</v>
       </c>
       <c r="M8">
-        <v>1.00632925262209</v>
+        <v>0.9863312710194294</v>
       </c>
       <c r="N8">
-        <v>1.004846184207845</v>
+        <v>0.9915345576543744</v>
       </c>
       <c r="O8">
-        <v>1.00729645739696</v>
+        <v>0.9784630782537093</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -690,34 +753,43 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>1.003939275538649</v>
+        <v>0.9897890356080422</v>
       </c>
       <c r="D9">
-        <v>1.006371017556539</v>
+        <v>0.9884632155952361</v>
       </c>
       <c r="E9">
-        <v>1.004900298689138</v>
+        <v>0.9921646160006153</v>
       </c>
       <c r="F9">
         <v>1</v>
       </c>
       <c r="G9">
-        <v>1.00734699784861</v>
+        <v>0.9819496678335841</v>
       </c>
       <c r="H9">
-        <v>1.007284843401909</v>
+        <v>0.9893607804275392</v>
+      </c>
+      <c r="I9">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J9">
+        <v>0.9887597948265848</v>
+      </c>
+      <c r="K9">
+        <v>0.9950272184133685</v>
       </c>
       <c r="L9">
-        <v>1.003892622293374</v>
+        <v>0.9872066241273124</v>
       </c>
       <c r="M9">
-        <v>1.006335295569792</v>
+        <v>0.9877763053471029</v>
       </c>
       <c r="N9">
-        <v>1.004853632042069</v>
+        <v>0.9931293024740582</v>
       </c>
       <c r="O9">
-        <v>1.007303497376133</v>
+        <v>0.9800701098586213</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -728,34 +800,43 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>1.00392547587129</v>
+        <v>0.9826119284642001</v>
       </c>
       <c r="D10">
-        <v>1.006329468373303</v>
+        <v>0.9771630686930983</v>
       </c>
       <c r="E10">
-        <v>1.004877172289456</v>
+        <v>0.9853521020509547</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G10">
-        <v>1.00725761292147</v>
+        <v>0.9631908147892677</v>
       </c>
       <c r="H10">
-        <v>1.007243256490323</v>
+        <v>0.9780503725320742</v>
+      </c>
+      <c r="I10">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J10">
+        <v>0.9774562574200464</v>
+      </c>
+      <c r="K10">
+        <v>0.9887492927963573</v>
       </c>
       <c r="L10">
-        <v>1.003881429308684</v>
+        <v>0.9806029195305277</v>
       </c>
       <c r="M10">
-        <v>1.00629100048322</v>
+        <v>0.9758145109284186</v>
       </c>
       <c r="N10">
-        <v>1.004833109832298</v>
+        <v>0.9868633513788228</v>
       </c>
       <c r="O10">
-        <v>1.00720589739475</v>
+        <v>0.9589924310616695</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -766,34 +847,43 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>1.00391978546473</v>
+        <v>0.9801251315318334</v>
       </c>
       <c r="D11">
-        <v>1.006318194511407</v>
+        <v>0.9737174816890366</v>
       </c>
       <c r="E11">
-        <v>1.004869580051885</v>
+        <v>0.9831088128833123</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11">
-        <v>1.007236707650867</v>
+        <v>0.9579094060441602</v>
       </c>
       <c r="H11">
-        <v>1.007231972391301</v>
+        <v>0.9746016567947702</v>
+      </c>
+      <c r="I11">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J11">
+        <v>0.9740096365995217</v>
+      </c>
+      <c r="K11">
+        <v>0.9864121498796796</v>
       </c>
       <c r="L11">
-        <v>1.003875413962635</v>
+        <v>0.9780329713119801</v>
       </c>
       <c r="M11">
-        <v>1.006279174341269</v>
+        <v>0.9722073077348008</v>
       </c>
       <c r="N11">
-        <v>1.004825193012253</v>
+        <v>0.9845306663309468</v>
       </c>
       <c r="O11">
-        <v>1.007183328522134</v>
+        <v>0.9531012161532055</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -804,34 +894,43 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>1.003930314575257</v>
+        <v>0.9866011721153686</v>
       </c>
       <c r="D12">
-        <v>1.006351329138321</v>
+        <v>0.9837971484161813</v>
       </c>
       <c r="E12">
-        <v>1.004887928850317</v>
+        <v>0.9892153305456723</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12">
-        <v>1.00730840833481</v>
+        <v>0.9746085993485624</v>
       </c>
       <c r="H12">
-        <v>1.007265137105806</v>
+        <v>0.9846904762695666</v>
+      </c>
+      <c r="I12">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J12">
+        <v>0.9840923276372964</v>
+      </c>
+      <c r="K12">
+        <v>0.9920856098494995</v>
       </c>
       <c r="L12">
-        <v>1.003883824776835</v>
+        <v>0.9840413789166247</v>
       </c>
       <c r="M12">
-        <v>1.006314522153495</v>
+        <v>0.9828726883309427</v>
       </c>
       <c r="N12">
-        <v>1.00484142553182</v>
+        <v>0.9901933047373881</v>
       </c>
       <c r="O12">
-        <v>1.007261672677335</v>
+        <v>0.9719317158919567</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -842,34 +941,43 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>1.003940629217264</v>
+        <v>0.9914852324653254</v>
       </c>
       <c r="D13">
-        <v>1.006382221134806</v>
+        <v>0.9912648626430132</v>
       </c>
       <c r="E13">
-        <v>1.004905875411483</v>
+        <v>0.9937859587676097</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>0.9999999999999997</v>
       </c>
       <c r="G13">
-        <v>1.007373592667182</v>
+        <v>0.986674038432259</v>
       </c>
       <c r="H13">
-        <v>1.007296057153481</v>
+        <v>0.9921649714848685</v>
+      </c>
+      <c r="I13">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J13">
+        <v>0.9915622824826057</v>
+      </c>
+      <c r="K13">
+        <v>0.9963984559869955</v>
       </c>
       <c r="L13">
-        <v>1.003892896644467</v>
+        <v>0.9886428515148532</v>
       </c>
       <c r="M13">
-        <v>1.006347383419999</v>
+        <v>0.9907481576604448</v>
       </c>
       <c r="N13">
-        <v>1.00485813048735</v>
+        <v>0.9944979245477278</v>
       </c>
       <c r="O13">
-        <v>1.007332717794951</v>
+        <v>0.9853351349085974</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -880,34 +988,43 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>1.003923704601197</v>
+        <v>0.9874433406938045</v>
       </c>
       <c r="D14">
-        <v>1.006364254054875</v>
+        <v>0.9872495954449433</v>
       </c>
       <c r="E14">
-        <v>1.004887932359954</v>
+        <v>0.9903533457556403</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14">
-        <v>1.007354842916043</v>
+        <v>0.9825303383729179</v>
       </c>
       <c r="H14">
-        <v>1.00727807375871</v>
+        <v>0.9881460582607529</v>
+      </c>
+      <c r="I14">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J14">
+        <v>0.9875458105408079</v>
+      </c>
+      <c r="K14">
+        <v>0.9914549780550801</v>
       </c>
       <c r="L14">
-        <v>1.003870770975987</v>
+        <v>0.9830938245858712</v>
       </c>
       <c r="M14">
-        <v>1.006329372954646</v>
+        <v>0.9867219790690366</v>
       </c>
       <c r="N14">
-        <v>1.004834991800214</v>
+        <v>0.9895638758107015</v>
       </c>
       <c r="O14">
-        <v>1.007313838369908</v>
+        <v>0.9811566432922906</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -918,34 +1035,43 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>1.003941529084153</v>
+        <v>0.9923527992991032</v>
       </c>
       <c r="D15">
-        <v>1.006385918106139</v>
+        <v>0.992361309056801</v>
       </c>
       <c r="E15">
-        <v>1.004908591217782</v>
+        <v>0.9945583359714845</v>
       </c>
       <c r="F15">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G15">
-        <v>1.007380780710666</v>
+        <v>0.9881819676922552</v>
       </c>
       <c r="H15">
-        <v>1.007299757481814</v>
+        <v>0.9932624135166275</v>
+      </c>
+      <c r="I15">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J15">
+        <v>0.9926590578749834</v>
+      </c>
+      <c r="K15">
+        <v>0.9972946518887379</v>
       </c>
       <c r="L15">
-        <v>1.003894254683897</v>
+        <v>0.9896312332750119</v>
       </c>
       <c r="M15">
-        <v>1.006351280897426</v>
+        <v>0.9918808349578688</v>
       </c>
       <c r="N15">
-        <v>1.004861303970468</v>
+        <v>0.9953924110444857</v>
       </c>
       <c r="O15">
-        <v>1.007340499906423</v>
+        <v>0.9869543838822524</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -956,34 +1082,43 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>1.003958341242218</v>
+        <v>0.9963332161159905</v>
       </c>
       <c r="D16">
-        <v>1.006412067319802</v>
+        <v>0.9972589630574911</v>
       </c>
       <c r="E16">
-        <v>1.004929333158029</v>
+        <v>0.9981675300023829</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16">
-        <v>1.007421866180745</v>
+        <v>0.9947178922364165</v>
       </c>
       <c r="H16">
-        <v>1.007325930440027</v>
+        <v>0.9981645147864948</v>
+      </c>
+      <c r="I16">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J16">
+        <v>0.9975581813713874</v>
+      </c>
+      <c r="K16">
+        <v>1.001699594839977</v>
       </c>
       <c r="L16">
-        <v>1.003914359108714</v>
+        <v>0.9943929646026743</v>
       </c>
       <c r="M16">
-        <v>1.006378287180498</v>
+        <v>0.9969218825945572</v>
       </c>
       <c r="N16">
-        <v>1.004885334740153</v>
+        <v>0.999788952003011</v>
       </c>
       <c r="O16">
-        <v>1.007384119720835</v>
+        <v>0.9939146661144467</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -994,34 +1129,43 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>1.003963969844581</v>
+        <v>0.9974500724858488</v>
       </c>
       <c r="D17">
-        <v>1.006421635101281</v>
+        <v>0.9987756254954264</v>
       </c>
       <c r="E17">
-        <v>1.004936320079838</v>
+        <v>0.9992287038255466</v>
       </c>
       <c r="F17">
         <v>0.9999999999999999</v>
       </c>
       <c r="G17">
-        <v>1.007438167719</v>
+        <v>0.9969069038750491</v>
       </c>
       <c r="H17">
-        <v>1.007335506909441</v>
+        <v>0.9996825544156555</v>
+      </c>
+      <c r="I17">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J17">
+        <v>0.9990752988698381</v>
+      </c>
+      <c r="K17">
+        <v>1.002912797241131</v>
       </c>
       <c r="L17">
-        <v>1.003920669339705</v>
+        <v>0.9956567791675009</v>
       </c>
       <c r="M17">
-        <v>1.006388241647302</v>
+        <v>0.9984969518749355</v>
       </c>
       <c r="N17">
-        <v>1.004893002571227</v>
+        <v>1.000999840340659</v>
       </c>
       <c r="O17">
-        <v>1.00740156153517</v>
+        <v>0.9962677088875616</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1032,34 +1176,43 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>1.003927699385468</v>
+        <v>0.9845670539985825</v>
       </c>
       <c r="D18">
-        <v>1.006336980864539</v>
+        <v>0.9798106712454032</v>
       </c>
       <c r="E18">
-        <v>1.004882181113896</v>
+        <v>0.987093069210654</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18">
-        <v>1.007272418967494</v>
+        <v>0.9671536092193526</v>
       </c>
       <c r="H18">
-        <v>1.007250775803206</v>
+        <v>0.9807003792152598</v>
+      </c>
+      <c r="I18">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J18">
+        <v>0.9801046543609714</v>
+      </c>
+      <c r="K18">
+        <v>0.9905843836833218</v>
       </c>
       <c r="L18">
-        <v>1.003884010063695</v>
+        <v>0.9826440001248464</v>
       </c>
       <c r="M18">
-        <v>1.006298931363665</v>
+        <v>0.978578306545616</v>
       </c>
       <c r="N18">
-        <v>1.00483847549235</v>
+        <v>0.9886949420115431</v>
       </c>
       <c r="O18">
-        <v>1.00722196119461</v>
+        <v>0.9633840497792517</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1070,34 +1223,43 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>1.003864727282216</v>
+        <v>0.9492824053062057</v>
       </c>
       <c r="D19">
-        <v>1.006221969058403</v>
+        <v>0.9340172462403051</v>
       </c>
       <c r="E19">
-        <v>1.004799100011345</v>
+        <v>0.9565060656078134</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G19">
-        <v>1.007071989736298</v>
+        <v>0.8998564340281798</v>
       </c>
       <c r="H19">
-        <v>1.007135659561669</v>
+        <v>0.9348653719163675</v>
+      </c>
+      <c r="I19">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J19">
+        <v>0.9342974894629013</v>
+      </c>
+      <c r="K19">
+        <v>0.957426355164789</v>
       </c>
       <c r="L19">
-        <v>1.003812885080185</v>
+        <v>0.9448901694080496</v>
       </c>
       <c r="M19">
-        <v>1.006179025971159</v>
+        <v>0.9309563505054248</v>
       </c>
       <c r="N19">
-        <v>1.004747249986358</v>
+        <v>0.9556001591506935</v>
       </c>
       <c r="O19">
-        <v>1.007006686963507</v>
+        <v>0.8884087971500502</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1108,34 +1270,43 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>1.003812073056186</v>
+        <v>0.917597626130035</v>
       </c>
       <c r="D20">
-        <v>1.006168460755879</v>
+        <v>0.9027194897537949</v>
       </c>
       <c r="E20">
-        <v>1.004742950946254</v>
+        <v>0.9320689858744271</v>
       </c>
       <c r="F20">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G20">
-        <v>1.007023053215267</v>
+        <v>0.8669606608930009</v>
       </c>
       <c r="H20">
-        <v>1.007082102671429</v>
+        <v>0.9035391957930828</v>
+      </c>
+      <c r="I20">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J20">
+        <v>0.9029903423744799</v>
+      </c>
+      <c r="K20">
+        <v>0.9241201716847359</v>
       </c>
       <c r="L20">
-        <v>1.003742004339667</v>
+        <v>0.9039826685193088</v>
       </c>
       <c r="M20">
-        <v>1.006125784813431</v>
+        <v>0.8995403708963997</v>
       </c>
       <c r="N20">
-        <v>1.004672893399546</v>
+        <v>0.9223575039192498</v>
       </c>
       <c r="O20">
-        <v>1.006958564322372</v>
+        <v>0.8548475557083314</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1146,34 +1317,43 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>1.003830582682983</v>
+        <v>0.9293500909875693</v>
       </c>
       <c r="D21">
-        <v>1.006185216216568</v>
+        <v>0.9138804091935714</v>
       </c>
       <c r="E21">
-        <v>1.004761745614443</v>
+        <v>0.9410640653957161</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G21">
-        <v>1.007035327200444</v>
+        <v>0.8778244172367532</v>
       </c>
       <c r="H21">
-        <v>1.007098873346758</v>
+        <v>0.9147102498019837</v>
+      </c>
+      <c r="I21">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J21">
+        <v>0.9141546105447466</v>
+      </c>
+      <c r="K21">
+        <v>0.9369952426816992</v>
       </c>
       <c r="L21">
-        <v>1.003767214626575</v>
+        <v>0.9198270535410128</v>
       </c>
       <c r="M21">
-        <v>1.006142281659211</v>
+        <v>0.9106735667638671</v>
       </c>
       <c r="N21">
-        <v>1.004698381625911</v>
+        <v>0.9352080169925575</v>
       </c>
       <c r="O21">
-        <v>1.006970048123127</v>
+        <v>0.8656173274125788</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1184,34 +1364,43 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>1.003857081253264</v>
+        <v>0.9407719281693283</v>
       </c>
       <c r="D22">
-        <v>1.006203990462071</v>
+        <v>0.9226243133512289</v>
       </c>
       <c r="E22">
-        <v>1.004787124777937</v>
+        <v>0.9490935098662225</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
-        <v>1.007038286905835</v>
+        <v>0.8823937265654027</v>
       </c>
       <c r="H22">
-        <v>1.007117664640041</v>
+        <v>0.9234620937805118</v>
+      </c>
+      <c r="I22">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J22">
+        <v>0.9229011382298486</v>
+      </c>
+      <c r="K22">
+        <v>0.9496949750233646</v>
       </c>
       <c r="L22">
-        <v>1.003804644319408</v>
+        <v>0.9360823254740485</v>
       </c>
       <c r="M22">
-        <v>1.006160147146861</v>
+        <v>0.9190840058107757</v>
       </c>
       <c r="N22">
-        <v>1.004734680657765</v>
+        <v>0.9478835258516989</v>
       </c>
       <c r="O22">
-        <v>1.006970222276023</v>
+        <v>0.8685842642186784</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1222,34 +1411,43 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>1.003877838597957</v>
+        <v>0.9509914511532186</v>
       </c>
       <c r="D23">
-        <v>1.006226248089217</v>
+        <v>0.9331867504943965</v>
       </c>
       <c r="E23">
-        <v>1.004809290490385</v>
+        <v>0.957000582092611</v>
       </c>
       <c r="F23">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G23">
-        <v>1.00706162811979</v>
+        <v>0.8944736197960667</v>
       </c>
       <c r="H23">
-        <v>1.007139942478018</v>
+        <v>0.9340341220465187</v>
+      </c>
+      <c r="I23">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J23">
+        <v>0.9334667445344373</v>
+      </c>
+      <c r="K23">
+        <v>0.9596381406166152</v>
       </c>
       <c r="L23">
-        <v>1.003831839199121</v>
+        <v>0.9483545814827352</v>
       </c>
       <c r="M23">
-        <v>1.006182464886183</v>
+        <v>0.9297614513280639</v>
       </c>
       <c r="N23">
-        <v>1.004763277458894</v>
+        <v>0.9578077258406753</v>
       </c>
       <c r="O23">
-        <v>1.006993749603113</v>
+        <v>0.8812764698440747</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1260,34 +1458,43 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>1.003893155279887</v>
+        <v>0.9559145884041806</v>
       </c>
       <c r="D24">
-        <v>1.006238822498895</v>
+        <v>0.9369990347425817</v>
       </c>
       <c r="E24">
-        <v>1.004824603476691</v>
+        <v>0.9603141152047258</v>
       </c>
       <c r="F24">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G24">
-        <v>1.007067846848079</v>
+        <v>0.8966637194674282</v>
       </c>
       <c r="H24">
-        <v>1.007152528305772</v>
+        <v>0.9378498680039694</v>
+      </c>
+      <c r="I24">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J24">
+        <v>0.9372801726231968</v>
+      </c>
+      <c r="K24">
+        <v>0.9642879752634341</v>
       </c>
       <c r="L24">
-        <v>1.003852992422307</v>
+        <v>0.9546190979063724</v>
       </c>
       <c r="M24">
-        <v>1.006194673690488</v>
+        <v>0.9334444465651944</v>
       </c>
       <c r="N24">
-        <v>1.004784421286283</v>
+        <v>0.9624486913881086</v>
       </c>
       <c r="O24">
-        <v>1.006998845521921</v>
+        <v>0.8828430588732281</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -1298,34 +1505,43 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <v>1.003906561202012</v>
+        <v>0.9627094657934155</v>
       </c>
       <c r="D25">
-        <v>1.006257524407835</v>
+        <v>0.9452807128533109</v>
       </c>
       <c r="E25">
-        <v>1.004840372568218</v>
+        <v>0.96599051929267</v>
       </c>
       <c r="F25">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="G25">
-        <v>1.007094637824014</v>
+        <v>0.9083447246465038</v>
       </c>
       <c r="H25">
-        <v>1.007171247196806</v>
+        <v>0.9461390662155049</v>
+      </c>
+      <c r="I25">
+        <v>1.00191104615943</v>
+      </c>
+      <c r="J25">
+        <v>0.945564335574727</v>
+      </c>
+      <c r="K25">
+        <v>0.970527862011329</v>
       </c>
       <c r="L25">
-        <v>1.003869481484849</v>
+        <v>0.961952397139046</v>
       </c>
       <c r="M25">
-        <v>1.006213837761794</v>
+        <v>0.9419924006876205</v>
       </c>
       <c r="N25">
-        <v>1.004803270503533</v>
+        <v>0.9686766761696058</v>
       </c>
       <c r="O25">
-        <v>1.007027057869232</v>
+        <v>0.8958561496377084</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lab3 done falta el report
</commit_message>
<xml_diff>
--- a/Lab3 - Timeseries powerflow/results/res_bus/vm_pu.xlsx
+++ b/Lab3 - Timeseries powerflow/results/res_bus/vm_pu.xlsx
@@ -424,43 +424,37 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.991412918452992</v>
+        <v>0.993979075244931</v>
       </c>
       <c r="D2">
-        <v>0.986601626550307</v>
+        <v>0.9949798479784844</v>
       </c>
       <c r="E2">
-        <v>0.992613680192833</v>
+        <v>0.9973540890848477</v>
       </c>
       <c r="F2">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0.974316325861903</v>
+        <v>0.9829071632654329</v>
       </c>
       <c r="H2">
-        <v>0.9874975009839858</v>
-      </c>
-      <c r="I2">
-        <v>1.00191104615943</v>
+        <v>0.9958833301782321</v>
       </c>
       <c r="J2">
-        <v>0.9868976472291071</v>
-      </c>
-      <c r="K2">
-        <v>0.997709920870801</v>
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>0.991071574230921</v>
+        <v>0.9936388026113527</v>
       </c>
       <c r="M2">
-        <v>0.9854014881851936</v>
+        <v>0.9937976562499454</v>
       </c>
       <c r="N2">
-        <v>0.9958068879420655</v>
+        <v>0.9970152127389644</v>
       </c>
       <c r="O2">
-        <v>0.9706684610392248</v>
+        <v>0.9793297702495547</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -471,43 +465,37 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.9927068647806099</v>
+        <v>0.993624471265469</v>
       </c>
       <c r="D3">
-        <v>0.9884466247576442</v>
+        <v>0.9950699066052769</v>
       </c>
       <c r="E3">
-        <v>0.9938326202608346</v>
+        <v>0.9974572912098776</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>0.9771696028160756</v>
+        <v>0.9839461463727678</v>
       </c>
       <c r="H3">
-        <v>0.9893441745247911</v>
-      </c>
-      <c r="I3">
-        <v>1.00191104615943</v>
+        <v>0.9959734705819233</v>
       </c>
       <c r="J3">
-        <v>0.9887431990110654</v>
-      </c>
-      <c r="K3">
-        <v>0.998983502820711</v>
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>0.992413460816302</v>
+        <v>0.9933313763553113</v>
       </c>
       <c r="M3">
-        <v>0.9873358439731758</v>
+        <v>0.9939720253226711</v>
       </c>
       <c r="N3">
-        <v>0.9970780406604551</v>
+        <v>0.9971654777130754</v>
       </c>
       <c r="O3">
-        <v>0.9738434027420182</v>
+        <v>0.9806699053221377</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -518,43 +506,37 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.9876275637982947</v>
+        <v>0.9949192836467563</v>
       </c>
       <c r="D4">
-        <v>0.9806856990150333</v>
+        <v>0.9945438180640228</v>
       </c>
       <c r="E4">
-        <v>0.9889005695763177</v>
+        <v>0.9971231989139545</v>
       </c>
       <c r="F4">
         <v>1</v>
       </c>
       <c r="G4">
-        <v>0.964521919088422</v>
+        <v>0.9788562563145931</v>
       </c>
       <c r="H4">
-        <v>0.98157620154572</v>
-      </c>
-      <c r="I4">
-        <v>1.00191104615943</v>
+        <v>0.9954469043308607</v>
       </c>
       <c r="J4">
-        <v>0.9809799446745778</v>
-      </c>
-      <c r="K4">
-        <v>0.9940227554399166</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9873324329905674</v>
+        <v>0.9946266233357345</v>
       </c>
       <c r="M4">
-        <v>0.9791433665504153</v>
+        <v>0.9930417482285482</v>
       </c>
       <c r="N4">
-        <v>0.9921267554143143</v>
+        <v>0.9968312743272536</v>
       </c>
       <c r="O4">
-        <v>0.9595980535122357</v>
+        <v>0.9740983416572403</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -565,43 +547,37 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.9880405230101313</v>
+        <v>0.9948378630038087</v>
       </c>
       <c r="D5">
-        <v>0.9813115129876749</v>
+        <v>0.994592133159213</v>
       </c>
       <c r="E5">
-        <v>0.9892982900713927</v>
+        <v>0.9971538814777505</v>
       </c>
       <c r="F5">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G5">
-        <v>0.9655416561908783</v>
+        <v>0.9792662085892417</v>
       </c>
       <c r="H5">
-        <v>0.9822025837829206</v>
-      </c>
-      <c r="I5">
-        <v>1.00191104615943</v>
+        <v>0.9954952632981243</v>
       </c>
       <c r="J5">
-        <v>0.981605946416905</v>
-      </c>
-      <c r="K5">
-        <v>0.9944227909938281</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="L5">
-        <v>0.987745533626158</v>
+        <v>0.9945451754158078</v>
       </c>
       <c r="M5">
-        <v>0.9798037843388554</v>
+        <v>0.9931219504702389</v>
       </c>
       <c r="N5">
-        <v>0.9925260279399992</v>
+        <v>0.9968619670981913</v>
       </c>
       <c r="O5">
-        <v>0.9607499660356039</v>
+        <v>0.9746285535069026</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -612,43 +588,37 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.9825674952481146</v>
+        <v>0.9948144376853374</v>
       </c>
       <c r="D6">
-        <v>0.9759489442219574</v>
+        <v>0.9944356278807013</v>
       </c>
       <c r="E6">
-        <v>0.9850001995921686</v>
+        <v>0.9961851265146134</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.9599594632248213</v>
+        <v>0.9790718602697165</v>
       </c>
       <c r="H6">
-        <v>0.9768351455864962</v>
-      </c>
-      <c r="I6">
-        <v>1.00191104615943</v>
+        <v>0.9953386159064495</v>
       </c>
       <c r="J6">
-        <v>0.9762417686621047</v>
-      </c>
-      <c r="K6">
-        <v>0.9890080593965691</v>
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9811754057837218</v>
+        <v>0.9934539069838949</v>
       </c>
       <c r="M6">
-        <v>0.974422529401186</v>
+        <v>0.9929621250551242</v>
       </c>
       <c r="N6">
-        <v>0.9871216244073553</v>
+        <v>0.9948280440691954</v>
       </c>
       <c r="O6">
-        <v>0.9550916407657314</v>
+        <v>0.974421573129465</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -659,43 +629,37 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.991011722163194</v>
+        <v>0.9917838238992799</v>
       </c>
       <c r="D7">
-        <v>0.9902495639652201</v>
+        <v>0.9953798144180316</v>
       </c>
       <c r="E7">
-        <v>0.9933027343024717</v>
+        <v>0.9959893392176188</v>
       </c>
       <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0.9899289126363155</v>
+      </c>
+      <c r="H7">
+        <v>0.9962836598035857</v>
+      </c>
+      <c r="J7">
         <v>0.9999999999999999</v>
       </c>
-      <c r="G7">
-        <v>0.984741140893128</v>
-      </c>
-      <c r="H7">
-        <v>0.9911487508745511</v>
-      </c>
-      <c r="I7">
-        <v>1.00191104615943</v>
-      </c>
-      <c r="J7">
-        <v>0.9905466791738494</v>
-      </c>
-      <c r="K7">
-        <v>0.996177732192194</v>
-      </c>
       <c r="L7">
-        <v>0.9884359867814143</v>
+        <v>0.989212288900464</v>
       </c>
       <c r="M7">
-        <v>0.9896517055774779</v>
+        <v>0.9947864902534364</v>
       </c>
       <c r="N7">
-        <v>0.9942776217617193</v>
+        <v>0.99344047531562</v>
       </c>
       <c r="O7">
-        <v>0.9831481071063324</v>
+        <v>0.9883517816410423</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -706,43 +670,37 @@
         <v>1</v>
       </c>
       <c r="C8">
-        <v>0.9883965474584619</v>
+        <v>0.992189047554438</v>
       </c>
       <c r="D8">
-        <v>0.9870300066223741</v>
+        <v>0.9952458554843827</v>
       </c>
       <c r="E8">
-        <v>0.9909931175490267</v>
+        <v>0.9956501536414539</v>
       </c>
       <c r="F8">
         <v>0.9999999999999999</v>
       </c>
       <c r="G8">
-        <v>0.9803816681823642</v>
+        <v>0.9887075956889463</v>
       </c>
       <c r="H8">
-        <v>0.9879262700425949</v>
-      </c>
-      <c r="I8">
-        <v>1.00191104615943</v>
+        <v>0.9961495792297728</v>
       </c>
       <c r="J8">
-        <v>0.9873261558326467</v>
-      </c>
-      <c r="K8">
-        <v>0.9934294259627219</v>
+        <v>1</v>
       </c>
       <c r="L8">
-        <v>0.9853903811192537</v>
+        <v>0.9892075475422283</v>
       </c>
       <c r="M8">
-        <v>0.9863312710194294</v>
+        <v>0.9945560078571282</v>
       </c>
       <c r="N8">
-        <v>0.9915345576543744</v>
+        <v>0.9926908638383636</v>
       </c>
       <c r="O8">
-        <v>0.9784630782537093</v>
+        <v>0.9868209137500574</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -753,43 +711,37 @@
         <v>1</v>
       </c>
       <c r="C9">
-        <v>0.9897890356080422</v>
+        <v>0.992194763370253</v>
       </c>
       <c r="D9">
-        <v>0.9884632155952361</v>
+        <v>0.9953111323942189</v>
       </c>
       <c r="E9">
-        <v>0.9921646160006153</v>
+        <v>0.9959464785928553</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G9">
-        <v>0.9819496678335841</v>
+        <v>0.9888875773188175</v>
       </c>
       <c r="H9">
-        <v>0.9893607804275392</v>
-      </c>
-      <c r="I9">
-        <v>1.00191104615943</v>
+        <v>0.9962149154137</v>
       </c>
       <c r="J9">
-        <v>0.9887597948265848</v>
-      </c>
-      <c r="K9">
-        <v>0.9950272184133685</v>
+        <v>0.9999999999999997</v>
       </c>
       <c r="L9">
-        <v>0.9872066241273124</v>
+        <v>0.9896254591078131</v>
       </c>
       <c r="M9">
-        <v>0.9877763053471029</v>
+        <v>0.9946314714659704</v>
       </c>
       <c r="N9">
-        <v>0.9931293024740582</v>
+        <v>0.9933973853939897</v>
       </c>
       <c r="O9">
-        <v>0.9800701098586213</v>
+        <v>0.9870339780230196</v>
       </c>
     </row>
     <row r="10" spans="1:15">
@@ -800,43 +752,37 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <v>0.9826119284642001</v>
+        <v>0.9942931649584107</v>
       </c>
       <c r="D10">
-        <v>0.9771630686930983</v>
+        <v>0.9945935665439163</v>
       </c>
       <c r="E10">
-        <v>0.9853521020509547</v>
+        <v>0.9958739819436905</v>
       </c>
       <c r="F10">
         <v>0.9999999999999999</v>
       </c>
       <c r="G10">
-        <v>0.9631908147892677</v>
+        <v>0.9811286363385037</v>
       </c>
       <c r="H10">
-        <v>0.9780503725320742</v>
-      </c>
-      <c r="I10">
-        <v>1.00191104615943</v>
+        <v>0.995496697984399</v>
       </c>
       <c r="J10">
-        <v>0.9774562574200464</v>
-      </c>
-      <c r="K10">
-        <v>0.9887492927963573</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="L10">
-        <v>0.9806029195305277</v>
+        <v>0.9923310422161266</v>
       </c>
       <c r="M10">
-        <v>0.9758145109284186</v>
+        <v>0.9932879257742934</v>
       </c>
       <c r="N10">
-        <v>0.9868633513788228</v>
+        <v>0.9939180536628169</v>
       </c>
       <c r="O10">
-        <v>0.9589924310616695</v>
+        <v>0.9771023998958911</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -847,43 +793,37 @@
         <v>1</v>
       </c>
       <c r="C11">
-        <v>0.9801251315318334</v>
+        <v>0.9945206118438148</v>
       </c>
       <c r="D11">
-        <v>0.9737174816890366</v>
+        <v>0.9943186432622969</v>
       </c>
       <c r="E11">
-        <v>0.9831088128833123</v>
+        <v>0.9956526852566987</v>
       </c>
       <c r="F11">
         <v>1</v>
       </c>
       <c r="G11">
-        <v>0.9579094060441602</v>
+        <v>0.979198060527379</v>
       </c>
       <c r="H11">
-        <v>0.9746016567947702</v>
-      </c>
-      <c r="I11">
-        <v>1.00191104615943</v>
+        <v>0.9952215250612498</v>
       </c>
       <c r="J11">
-        <v>0.9740096365995217</v>
-      </c>
-      <c r="K11">
-        <v>0.9864121498796796</v>
+        <v>1</v>
       </c>
       <c r="L11">
-        <v>0.9780329713119801</v>
+        <v>0.9924889730402187</v>
       </c>
       <c r="M11">
-        <v>0.9722073077348008</v>
+        <v>0.9928666145481658</v>
       </c>
       <c r="N11">
-        <v>0.9845306663309468</v>
+        <v>0.9936256733170646</v>
       </c>
       <c r="O11">
-        <v>0.9531012161532055</v>
+        <v>0.9746283578002397</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -894,43 +834,37 @@
         <v>1</v>
       </c>
       <c r="C12">
-        <v>0.9866011721153686</v>
+        <v>0.993083787769835</v>
       </c>
       <c r="D12">
-        <v>0.9837971484161813</v>
+        <v>0.9950733431778213</v>
       </c>
       <c r="E12">
-        <v>0.9892153305456723</v>
+        <v>0.9958207131780678</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="G12">
-        <v>0.9746085993485624</v>
+        <v>0.9860941143927945</v>
       </c>
       <c r="H12">
-        <v>0.9846904762695666</v>
-      </c>
-      <c r="I12">
-        <v>1.00191104615943</v>
+        <v>0.9959769102750152</v>
       </c>
       <c r="J12">
-        <v>0.9840923276372964</v>
-      </c>
-      <c r="K12">
-        <v>0.9920856098494995</v>
+        <v>1</v>
       </c>
       <c r="L12">
-        <v>0.9840413789166247</v>
+        <v>0.9905588212844966</v>
       </c>
       <c r="M12">
-        <v>0.9828726883309427</v>
+        <v>0.9941662994377274</v>
       </c>
       <c r="N12">
-        <v>0.9901933047373881</v>
+        <v>0.993310203424481</v>
       </c>
       <c r="O12">
-        <v>0.9719317158919567</v>
+        <v>0.9834825857359527</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -941,43 +875,37 @@
         <v>1</v>
       </c>
       <c r="C13">
-        <v>0.9914852324653254</v>
+        <v>0.9912600423546456</v>
       </c>
       <c r="D13">
-        <v>0.9912648626430132</v>
+        <v>0.9953689591844146</v>
       </c>
       <c r="E13">
-        <v>0.9937859587676097</v>
+        <v>0.9958188919924562</v>
       </c>
       <c r="F13">
-        <v>0.9999999999999997</v>
+        <v>1</v>
       </c>
       <c r="G13">
-        <v>0.986674038432259</v>
+        <v>0.9908171618147896</v>
       </c>
       <c r="H13">
-        <v>0.9921649714848685</v>
-      </c>
-      <c r="I13">
-        <v>1.00191104615943</v>
+        <v>0.996272794712975</v>
       </c>
       <c r="J13">
-        <v>0.9915622824826057</v>
-      </c>
-      <c r="K13">
-        <v>0.9963984559869955</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="L13">
-        <v>0.9886428515148532</v>
+        <v>0.9884162843909573</v>
       </c>
       <c r="M13">
-        <v>0.9907481576604448</v>
+        <v>0.9948552458847431</v>
       </c>
       <c r="N13">
-        <v>0.9944979245477278</v>
+        <v>0.99300278905879</v>
       </c>
       <c r="O13">
-        <v>0.9853351349085974</v>
+        <v>0.9894885316301043</v>
       </c>
     </row>
     <row r="14" spans="1:15">
@@ -988,43 +916,37 @@
         <v>1</v>
       </c>
       <c r="C14">
-        <v>0.9874433406938045</v>
+        <v>0.9910473724789013</v>
       </c>
       <c r="D14">
-        <v>0.9872495954449433</v>
+        <v>0.9951476542302997</v>
       </c>
       <c r="E14">
-        <v>0.9903533457556403</v>
+        <v>0.9948155183826323</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14">
-        <v>0.9825303383729179</v>
+        <v>0.9905052367312093</v>
       </c>
       <c r="H14">
-        <v>0.9881460582607529</v>
-      </c>
-      <c r="I14">
-        <v>1.00191104615943</v>
+        <v>0.9960512888049539</v>
       </c>
       <c r="J14">
-        <v>0.9875458105408079</v>
-      </c>
-      <c r="K14">
-        <v>0.9914549780550801</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="L14">
-        <v>0.9830938245858712</v>
+        <v>0.9867338485001819</v>
       </c>
       <c r="M14">
-        <v>0.9867219790690366</v>
+        <v>0.9946259531284898</v>
       </c>
       <c r="N14">
-        <v>0.9895638758107015</v>
+        <v>0.9905391020553729</v>
       </c>
       <c r="O14">
-        <v>0.9811566432922906</v>
+        <v>0.9891519136333979</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -1035,43 +957,37 @@
         <v>1</v>
       </c>
       <c r="C15">
-        <v>0.9923527992991032</v>
+        <v>0.9910122741661758</v>
       </c>
       <c r="D15">
-        <v>0.992361309056801</v>
+        <v>0.9953816720402139</v>
       </c>
       <c r="E15">
-        <v>0.9945583359714845</v>
+        <v>0.9958997106843204</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15">
-        <v>0.9881819676922552</v>
+        <v>0.991228815928906</v>
       </c>
       <c r="H15">
-        <v>0.9932624135166275</v>
-      </c>
-      <c r="I15">
-        <v>1.00191104615943</v>
+        <v>0.9962855191125647</v>
       </c>
       <c r="J15">
-        <v>0.9926590578749834</v>
-      </c>
-      <c r="K15">
-        <v>0.9972946518887379</v>
+        <v>1</v>
       </c>
       <c r="L15">
-        <v>0.9896312332750119</v>
+        <v>0.9882829098628939</v>
       </c>
       <c r="M15">
-        <v>0.9918808349578688</v>
+        <v>0.9949031959108006</v>
       </c>
       <c r="N15">
-        <v>0.9953924110444857</v>
+        <v>0.993198593533112</v>
       </c>
       <c r="O15">
-        <v>0.9869543838822524</v>
+        <v>0.9900080232009912</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1082,43 +998,37 @@
         <v>1</v>
       </c>
       <c r="C16">
-        <v>0.9963332161159905</v>
+        <v>0.9898648861266423</v>
       </c>
       <c r="D16">
-        <v>0.9972589630574911</v>
+        <v>0.995418453217066</v>
       </c>
       <c r="E16">
-        <v>0.9981675300023829</v>
+        <v>0.9964109003453668</v>
       </c>
       <c r="F16">
         <v>1</v>
       </c>
       <c r="G16">
-        <v>0.9947178922364165</v>
+        <v>0.9928663990099267</v>
       </c>
       <c r="H16">
-        <v>0.9981645147864948</v>
-      </c>
-      <c r="I16">
-        <v>1.00191104615943</v>
+        <v>0.9963223336882226</v>
       </c>
       <c r="J16">
-        <v>0.9975581813713874</v>
-      </c>
-      <c r="K16">
-        <v>1.001699594839977</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="L16">
-        <v>0.9943929646026743</v>
+        <v>0.9878993229734896</v>
       </c>
       <c r="M16">
-        <v>0.9969218825945572</v>
+        <v>0.9950806251766237</v>
       </c>
       <c r="N16">
-        <v>0.999788952003011</v>
+        <v>0.9944709492595286</v>
       </c>
       <c r="O16">
-        <v>0.9939146661144467</v>
+        <v>0.9920607474815649</v>
       </c>
     </row>
     <row r="17" spans="1:15">
@@ -1129,43 +1039,37 @@
         <v>1</v>
       </c>
       <c r="C17">
-        <v>0.9974500724858488</v>
+        <v>0.9892884398954911</v>
       </c>
       <c r="D17">
-        <v>0.9987756254954264</v>
+        <v>0.9953851572537726</v>
       </c>
       <c r="E17">
-        <v>0.9992287038255466</v>
+        <v>0.996485320239295</v>
       </c>
       <c r="F17">
+        <v>0.9999999999999998</v>
+      </c>
+      <c r="G17">
+        <v>0.9934998378097286</v>
+      </c>
+      <c r="H17">
+        <v>0.9962890074908392</v>
+      </c>
+      <c r="J17">
         <v>0.9999999999999999</v>
       </c>
-      <c r="G17">
-        <v>0.9969069038750491</v>
-      </c>
-      <c r="H17">
-        <v>0.9996825544156555</v>
-      </c>
-      <c r="I17">
-        <v>1.00191104615943</v>
-      </c>
-      <c r="J17">
-        <v>0.9990752988698381</v>
-      </c>
-      <c r="K17">
-        <v>1.002912797241131</v>
-      </c>
       <c r="L17">
-        <v>0.9956567791675009</v>
+        <v>0.9874660410856098</v>
       </c>
       <c r="M17">
-        <v>0.9984969518749355</v>
+        <v>0.9951054367543352</v>
       </c>
       <c r="N17">
-        <v>1.000999840340659</v>
+        <v>0.994688630587452</v>
       </c>
       <c r="O17">
-        <v>0.9962677088875616</v>
+        <v>0.9928573187592444</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -1176,43 +1080,37 @@
         <v>1</v>
       </c>
       <c r="C18">
-        <v>0.9845670539985825</v>
+        <v>0.9940477591681391</v>
       </c>
       <c r="D18">
-        <v>0.9798106712454032</v>
+        <v>0.9947691887379668</v>
       </c>
       <c r="E18">
-        <v>0.987093069210654</v>
+        <v>0.9960381552244415</v>
       </c>
       <c r="F18">
         <v>1</v>
       </c>
       <c r="G18">
-        <v>0.9671536092193526</v>
+        <v>0.9825029202106044</v>
       </c>
       <c r="H18">
-        <v>0.9807003792152598</v>
-      </c>
-      <c r="I18">
-        <v>1.00191104615943</v>
+        <v>0.9956724796505496</v>
       </c>
       <c r="J18">
-        <v>0.9801046543609714</v>
-      </c>
-      <c r="K18">
-        <v>0.9905843836833218</v>
+        <v>0.9999999999999998</v>
       </c>
       <c r="L18">
-        <v>0.9826440001248464</v>
+        <v>0.9921608821781657</v>
       </c>
       <c r="M18">
-        <v>0.978578306545616</v>
+        <v>0.9935698323709092</v>
       </c>
       <c r="N18">
-        <v>0.9886949420115431</v>
+        <v>0.9941587177363297</v>
       </c>
       <c r="O18">
-        <v>0.9633840497792517</v>
+        <v>0.9788635525865069</v>
       </c>
     </row>
     <row r="19" spans="1:15">
@@ -1223,43 +1121,37 @@
         <v>1</v>
       </c>
       <c r="C19">
-        <v>0.9492824053062057</v>
+        <v>0.9929467789631036</v>
       </c>
       <c r="D19">
-        <v>0.9340172462403051</v>
+        <v>0.9906928642665799</v>
       </c>
       <c r="E19">
-        <v>0.9565060656078134</v>
+        <v>0.9921593072185186</v>
       </c>
       <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0.9611089559593372</v>
+      </c>
+      <c r="H19">
+        <v>0.9915924537106279</v>
+      </c>
+      <c r="J19">
         <v>0.9999999999999999</v>
       </c>
-      <c r="G19">
-        <v>0.8998564340281798</v>
-      </c>
-      <c r="H19">
-        <v>0.9348653719163675</v>
-      </c>
-      <c r="I19">
-        <v>1.00191104615943</v>
-      </c>
-      <c r="J19">
-        <v>0.9342974894629013</v>
-      </c>
-      <c r="K19">
-        <v>0.957426355164789</v>
-      </c>
       <c r="L19">
-        <v>0.9448901694080496</v>
+        <v>0.9889815787837511</v>
       </c>
       <c r="M19">
-        <v>0.9309563505054248</v>
+        <v>0.987994548666092</v>
       </c>
       <c r="N19">
-        <v>0.9556001591506935</v>
+        <v>0.9881870229875505</v>
       </c>
       <c r="O19">
-        <v>0.8884087971500502</v>
+        <v>0.9514546711419518</v>
       </c>
     </row>
     <row r="20" spans="1:15">
@@ -1270,43 +1162,37 @@
         <v>1</v>
       </c>
       <c r="C20">
-        <v>0.917597626130035</v>
+        <v>0.9857287020906186</v>
       </c>
       <c r="D20">
-        <v>0.9027194897537949</v>
+        <v>0.9880009352247359</v>
       </c>
       <c r="E20">
-        <v>0.9320689858744271</v>
+        <v>0.9866423475669851</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
-        <v>0.8669606608930009</v>
+        <v>0.9593582825552284</v>
       </c>
       <c r="H20">
-        <v>0.9035391957930828</v>
-      </c>
-      <c r="I20">
-        <v>1.00191104615943</v>
+        <v>0.9888980802876466</v>
       </c>
       <c r="J20">
-        <v>0.9029903423744799</v>
-      </c>
-      <c r="K20">
-        <v>0.9241201716847359</v>
+        <v>1</v>
       </c>
       <c r="L20">
-        <v>0.9039826685193088</v>
+        <v>0.9744540606998332</v>
       </c>
       <c r="M20">
-        <v>0.8995403708963997</v>
+        <v>0.9853821903594211</v>
       </c>
       <c r="N20">
-        <v>0.9223575039192498</v>
+        <v>0.9753947335359675</v>
       </c>
       <c r="O20">
-        <v>0.8548475557083314</v>
+        <v>0.9500463009699752</v>
       </c>
     </row>
     <row r="21" spans="1:15">
@@ -1317,43 +1203,37 @@
         <v>1</v>
       </c>
       <c r="C21">
-        <v>0.9293500909875693</v>
+        <v>0.9887036047845105</v>
       </c>
       <c r="D21">
-        <v>0.9138804091935714</v>
+        <v>0.9889753876248141</v>
       </c>
       <c r="E21">
-        <v>0.9410640653957161</v>
+        <v>0.9888106941146061</v>
       </c>
       <c r="F21">
         <v>0.9999999999999999</v>
       </c>
       <c r="G21">
-        <v>0.8778244172367532</v>
+        <v>0.9593023735143466</v>
       </c>
       <c r="H21">
-        <v>0.9147102498019837</v>
-      </c>
-      <c r="I21">
-        <v>1.00191104615943</v>
+        <v>0.9898734175301662</v>
       </c>
       <c r="J21">
-        <v>0.9141546105447466</v>
-      </c>
-      <c r="K21">
-        <v>0.9369952426816992</v>
+        <v>1</v>
       </c>
       <c r="L21">
-        <v>0.9198270535410128</v>
+        <v>0.9805567510029491</v>
       </c>
       <c r="M21">
-        <v>0.9106735667638671</v>
+        <v>0.9862699954633181</v>
       </c>
       <c r="N21">
-        <v>0.9352080169925575</v>
+        <v>0.9806660341108467</v>
       </c>
       <c r="O21">
-        <v>0.8656173274125788</v>
+        <v>0.9496131417852303</v>
       </c>
     </row>
     <row r="22" spans="1:15">
@@ -1364,43 +1244,37 @@
         <v>1</v>
       </c>
       <c r="C22">
-        <v>0.9407719281693283</v>
+        <v>0.9922265071497063</v>
       </c>
       <c r="D22">
-        <v>0.9226243133512289</v>
+        <v>0.9896294137836643</v>
       </c>
       <c r="E22">
-        <v>0.9490935098662225</v>
+        <v>0.9913736146325236</v>
       </c>
       <c r="F22">
         <v>1</v>
       </c>
       <c r="G22">
-        <v>0.8823937265654027</v>
+        <v>0.9559664842551042</v>
       </c>
       <c r="H22">
-        <v>0.9234620937805118</v>
-      </c>
-      <c r="I22">
-        <v>1.00191104615943</v>
+        <v>0.9905280375713889</v>
       </c>
       <c r="J22">
-        <v>0.9229011382298486</v>
-      </c>
-      <c r="K22">
-        <v>0.9496949750233646</v>
+        <v>1</v>
       </c>
       <c r="L22">
-        <v>0.9360823254740485</v>
+        <v>0.9880763395477189</v>
       </c>
       <c r="M22">
-        <v>0.9190840058107757</v>
+        <v>0.9865929695426309</v>
       </c>
       <c r="N22">
-        <v>0.9478835258516989</v>
+        <v>0.9872153530177266</v>
       </c>
       <c r="O22">
-        <v>0.8685842642186784</v>
+        <v>0.9447938646892488</v>
       </c>
     </row>
     <row r="23" spans="1:15">
@@ -1411,43 +1285,37 @@
         <v>1</v>
       </c>
       <c r="C23">
-        <v>0.9509914511532186</v>
+        <v>0.9941299732920263</v>
       </c>
       <c r="D23">
-        <v>0.9331867504943965</v>
+        <v>0.9904691482753921</v>
       </c>
       <c r="E23">
-        <v>0.957000582092611</v>
+        <v>0.992959334455772</v>
       </c>
       <c r="F23">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G23">
-        <v>0.8944736197960667</v>
+        <v>0.957153793920178</v>
       </c>
       <c r="H23">
-        <v>0.9340341220465187</v>
-      </c>
-      <c r="I23">
-        <v>1.00191104615943</v>
+        <v>0.9913685345762143</v>
       </c>
       <c r="J23">
-        <v>0.9334667445344373</v>
-      </c>
-      <c r="K23">
-        <v>0.9596381406166152</v>
+        <v>1</v>
       </c>
       <c r="L23">
-        <v>0.9483545814827352</v>
+        <v>0.9917270766103421</v>
       </c>
       <c r="M23">
-        <v>0.9297614513280639</v>
+        <v>0.9874610559346365</v>
       </c>
       <c r="N23">
-        <v>0.9578077258406753</v>
+        <v>0.9905505710266135</v>
       </c>
       <c r="O23">
-        <v>0.8812764698440747</v>
+        <v>0.9461128576079337</v>
       </c>
     </row>
     <row r="24" spans="1:15">
@@ -1458,43 +1326,37 @@
         <v>1</v>
       </c>
       <c r="C24">
-        <v>0.9559145884041806</v>
+        <v>0.995247532258513</v>
       </c>
       <c r="D24">
-        <v>0.9369990347425817</v>
+        <v>0.9906197926260227</v>
       </c>
       <c r="E24">
-        <v>0.9603141152047258</v>
+        <v>0.9938711278553529</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
       <c r="G24">
-        <v>0.8966637194674282</v>
+        <v>0.9556219444886158</v>
       </c>
       <c r="H24">
-        <v>0.9378498680039694</v>
-      </c>
-      <c r="I24">
-        <v>1.00191104615943</v>
+        <v>0.991519315718047</v>
       </c>
       <c r="J24">
-        <v>0.9372801726231968</v>
-      </c>
-      <c r="K24">
-        <v>0.9642879752634341</v>
+        <v>1</v>
       </c>
       <c r="L24">
-        <v>0.9546190979063724</v>
+        <v>0.9940435336590371</v>
       </c>
       <c r="M24">
-        <v>0.9334444465651944</v>
+        <v>0.9874737522007472</v>
       </c>
       <c r="N24">
-        <v>0.9624486913881086</v>
+        <v>0.9926641372389237</v>
       </c>
       <c r="O24">
-        <v>0.8828430588732281</v>
+        <v>0.9439478778856533</v>
       </c>
     </row>
     <row r="25" spans="1:15">
@@ -1505,43 +1367,37 @@
         <v>1</v>
       </c>
       <c r="C25">
-        <v>0.9627094657934155</v>
+        <v>0.9958736075553308</v>
       </c>
       <c r="D25">
-        <v>0.9452807128533109</v>
+        <v>0.9913165407382651</v>
       </c>
       <c r="E25">
-        <v>0.96599051929267</v>
+        <v>0.9946920874470705</v>
       </c>
       <c r="F25">
-        <v>0.9999999999999998</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="G25">
-        <v>0.9083447246465038</v>
+        <v>0.9585123290777529</v>
       </c>
       <c r="H25">
-        <v>0.9461390662155049</v>
-      </c>
-      <c r="I25">
-        <v>1.00191104615943</v>
+        <v>0.9922166965059341</v>
       </c>
       <c r="J25">
-        <v>0.945564335574727</v>
-      </c>
-      <c r="K25">
-        <v>0.970527862011329</v>
+        <v>0.9999999999999999</v>
       </c>
       <c r="L25">
-        <v>0.961952397139046</v>
+        <v>0.9951561264273685</v>
       </c>
       <c r="M25">
-        <v>0.9419924006876205</v>
+        <v>0.9883503458902334</v>
       </c>
       <c r="N25">
-        <v>0.9686766761696058</v>
+        <v>0.9939732705840985</v>
       </c>
       <c r="O25">
-        <v>0.8958561496377084</v>
+        <v>0.9476640323827289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lab3 problem solved, ahora si que si
por algun motivo el csv con los perfiles de 24 horas se modificó
</commit_message>
<xml_diff>
--- a/Lab3 - Timeseries powerflow/results/res_bus/vm_pu.xlsx
+++ b/Lab3 - Timeseries powerflow/results/res_bus/vm_pu.xlsx
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -418,230 +418,986 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.9269129435096656</v>
+        <v>0.993979075244931</v>
       </c>
       <c r="D2">
-        <v>0.9024812690245277</v>
+        <v>0.9949798479784844</v>
       </c>
       <c r="E2">
-        <v>0.9317084155966886</v>
+        <v>0.9973540890848477</v>
       </c>
       <c r="F2">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G2">
-        <v>0.8556787029121204</v>
+        <v>0.9829071632654329</v>
       </c>
       <c r="H2">
-        <v>0.9033007587496975</v>
+        <v>0.9958833301782321</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
       </c>
       <c r="L2">
-        <v>0.9205662423618785</v>
+        <v>0.9936388026113527</v>
       </c>
       <c r="M2">
-        <v>0.8984492008720295</v>
+        <v>0.9937976562499454</v>
       </c>
       <c r="N2">
-        <v>0.9186365395054665</v>
+        <v>0.9970152127389644</v>
       </c>
       <c r="O2">
-        <v>0.8392124395714362</v>
+        <v>0.9793297702495547</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>0.9517003557980153</v>
+        <v>0.993624471265469</v>
       </c>
       <c r="D3">
-        <v>0.9289218689480673</v>
+        <v>0.9950699066052769</v>
       </c>
       <c r="E3">
-        <v>0.9467811712390947</v>
+        <v>0.9974572912098776</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>0.8856794480710755</v>
+        <v>0.9839461463727678</v>
       </c>
       <c r="H3">
-        <v>0.9297653678141559</v>
+        <v>0.9959734705819233</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
       </c>
       <c r="L3">
-        <v>0.9404372005809997</v>
+        <v>0.9933313763553113</v>
       </c>
       <c r="M3">
-        <v>0.9251451413302529</v>
+        <v>0.9939720253226711</v>
       </c>
       <c r="N3">
-        <v>0.9342532001591218</v>
+        <v>0.9971654777130754</v>
       </c>
       <c r="O3">
-        <v>0.8706992738723965</v>
+        <v>0.9806699053221377</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
-        <v>0.9605093481560002</v>
+        <v>0.9949192836467563</v>
       </c>
       <c r="D4">
-        <v>0.9322805671894684</v>
+        <v>0.9945438180640228</v>
       </c>
       <c r="E4">
-        <v>0.9457473874955494</v>
+        <v>0.9971231989139545</v>
       </c>
       <c r="F4">
-        <v>0.9999999999999999</v>
+        <v>1</v>
       </c>
       <c r="G4">
-        <v>0.8894550928965316</v>
+        <v>0.9788562563145931</v>
       </c>
       <c r="H4">
-        <v>0.9331271158902661</v>
+        <v>0.9954469043308607</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>0.9520401149732997</v>
+        <v>0.9946266233357345</v>
       </c>
       <c r="M4">
-        <v>0.9285343496383645</v>
+        <v>0.9930417482285482</v>
       </c>
       <c r="N4">
-        <v>0.9331832420325429</v>
+        <v>0.9968312743272536</v>
       </c>
       <c r="O4">
-        <v>0.874647191262057</v>
+        <v>0.9740983416572403</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5">
-        <v>0.9576805593621294</v>
+        <v>0.9948378630038087</v>
       </c>
       <c r="D5">
-        <v>0.9307742244533254</v>
+        <v>0.994592133159213</v>
       </c>
       <c r="E5">
-        <v>0.9450461123863778</v>
+        <v>0.9971538814777505</v>
       </c>
       <c r="F5">
         <v>0.9999999999999999</v>
       </c>
       <c r="G5">
-        <v>0.8877626618277507</v>
+        <v>0.9792662085892417</v>
       </c>
       <c r="H5">
-        <v>0.9316194053336075</v>
+        <v>0.9954952632981243</v>
+      </c>
+      <c r="J5">
+        <v>0.9999999999999998</v>
       </c>
       <c r="L5">
-        <v>0.9468078592514227</v>
+        <v>0.9945451754158078</v>
       </c>
       <c r="M5">
-        <v>0.9270143744335817</v>
+        <v>0.9931219504702389</v>
       </c>
       <c r="N5">
-        <v>0.9324573354439786</v>
+        <v>0.9968619670981913</v>
       </c>
       <c r="O5">
-        <v>0.8728779193888087</v>
+        <v>0.9746285535069026</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.949496309793167</v>
+        <v>0.9948144376853374</v>
       </c>
       <c r="D6">
-        <v>0.9274140339283574</v>
+        <v>0.9944356278807013</v>
       </c>
       <c r="E6">
-        <v>0.946058690095701</v>
+        <v>0.9961851265146134</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="G6">
-        <v>0.8839820214295047</v>
+        <v>0.9790718602697165</v>
       </c>
       <c r="H6">
-        <v>0.9282561636188761</v>
+        <v>0.9953386159064495</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
       </c>
       <c r="L6">
-        <v>0.9372874655544191</v>
+        <v>0.9934539069838949</v>
       </c>
       <c r="M6">
-        <v>0.92362347438861</v>
+        <v>0.9929621250551242</v>
       </c>
       <c r="N6">
-        <v>0.9335054548300317</v>
+        <v>0.9948280440691954</v>
       </c>
       <c r="O6">
-        <v>0.868923388055747</v>
+        <v>0.974421573129465</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0.9917838238992799</v>
+      </c>
+      <c r="D7">
+        <v>0.9953798144180316</v>
+      </c>
+      <c r="E7">
+        <v>0.9959893392176188</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0.9899289126363155</v>
+      </c>
+      <c r="H7">
+        <v>0.9962836598035857</v>
+      </c>
+      <c r="J7">
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="L7">
+        <v>0.989212288900464</v>
+      </c>
+      <c r="M7">
+        <v>0.9947864902534364</v>
+      </c>
+      <c r="N7">
+        <v>0.99344047531562</v>
+      </c>
+      <c r="O7">
+        <v>0.9883517816410423</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>0.9323315036332418</v>
-      </c>
-      <c r="D7">
-        <v>0.908548825803716</v>
-      </c>
-      <c r="E7">
-        <v>0.9356416896922236</v>
-      </c>
-      <c r="F7">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0.992189047554438</v>
+      </c>
+      <c r="D8">
+        <v>0.9952458554843827</v>
+      </c>
+      <c r="E8">
+        <v>0.9956501536414539</v>
+      </c>
+      <c r="F8">
         <v>0.9999999999999999</v>
       </c>
-      <c r="G7">
-        <v>0.8626098391670529</v>
-      </c>
-      <c r="H7">
-        <v>0.9093738251174037</v>
-      </c>
-      <c r="L7">
-        <v>0.9257451953567312</v>
-      </c>
-      <c r="M7">
-        <v>0.9045778343145603</v>
-      </c>
-      <c r="N7">
-        <v>0.9227152258673225</v>
-      </c>
-      <c r="O7">
-        <v>0.8465065138375081</v>
+      <c r="G8">
+        <v>0.9887075956889463</v>
+      </c>
+      <c r="H8">
+        <v>0.9961495792297728</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <v>0.9892075475422283</v>
+      </c>
+      <c r="M8">
+        <v>0.9945560078571282</v>
+      </c>
+      <c r="N8">
+        <v>0.9926908638383636</v>
+      </c>
+      <c r="O8">
+        <v>0.9868209137500574</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>0.992194763370253</v>
+      </c>
+      <c r="D9">
+        <v>0.9953111323942189</v>
+      </c>
+      <c r="E9">
+        <v>0.9959464785928553</v>
+      </c>
+      <c r="F9">
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="G9">
+        <v>0.9888875773188175</v>
+      </c>
+      <c r="H9">
+        <v>0.9962149154137</v>
+      </c>
+      <c r="J9">
+        <v>0.9999999999999997</v>
+      </c>
+      <c r="L9">
+        <v>0.9896254591078131</v>
+      </c>
+      <c r="M9">
+        <v>0.9946314714659704</v>
+      </c>
+      <c r="N9">
+        <v>0.9933973853939897</v>
+      </c>
+      <c r="O9">
+        <v>0.9870339780230196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0.9942931649584107</v>
+      </c>
+      <c r="D10">
+        <v>0.9945935665439163</v>
+      </c>
+      <c r="E10">
+        <v>0.9958739819436905</v>
+      </c>
+      <c r="F10">
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="G10">
+        <v>0.9811286363385037</v>
+      </c>
+      <c r="H10">
+        <v>0.995496697984399</v>
+      </c>
+      <c r="J10">
+        <v>0.9999999999999998</v>
+      </c>
+      <c r="L10">
+        <v>0.9923310422161266</v>
+      </c>
+      <c r="M10">
+        <v>0.9932879257742934</v>
+      </c>
+      <c r="N10">
+        <v>0.9939180536628169</v>
+      </c>
+      <c r="O10">
+        <v>0.9771023998958911</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0.9945206118438148</v>
+      </c>
+      <c r="D11">
+        <v>0.9943186432622969</v>
+      </c>
+      <c r="E11">
+        <v>0.9956526852566987</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0.979198060527379</v>
+      </c>
+      <c r="H11">
+        <v>0.9952215250612498</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="L11">
+        <v>0.9924889730402187</v>
+      </c>
+      <c r="M11">
+        <v>0.9928666145481658</v>
+      </c>
+      <c r="N11">
+        <v>0.9936256733170646</v>
+      </c>
+      <c r="O11">
+        <v>0.9746283578002397</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0.993083787769835</v>
+      </c>
+      <c r="D12">
+        <v>0.9950733431778213</v>
+      </c>
+      <c r="E12">
+        <v>0.9958207131780678</v>
+      </c>
+      <c r="F12">
+        <v>0.9999999999999998</v>
+      </c>
+      <c r="G12">
+        <v>0.9860941143927945</v>
+      </c>
+      <c r="H12">
+        <v>0.9959769102750152</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0.9905588212844966</v>
+      </c>
+      <c r="M12">
+        <v>0.9941662994377274</v>
+      </c>
+      <c r="N12">
+        <v>0.993310203424481</v>
+      </c>
+      <c r="O12">
+        <v>0.9834825857359527</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0.9912600423546456</v>
+      </c>
+      <c r="D13">
+        <v>0.9953689591844146</v>
+      </c>
+      <c r="E13">
+        <v>0.9958188919924562</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0.9908171618147896</v>
+      </c>
+      <c r="H13">
+        <v>0.996272794712975</v>
+      </c>
+      <c r="J13">
+        <v>0.9999999999999998</v>
+      </c>
+      <c r="L13">
+        <v>0.9884162843909573</v>
+      </c>
+      <c r="M13">
+        <v>0.9948552458847431</v>
+      </c>
+      <c r="N13">
+        <v>0.99300278905879</v>
+      </c>
+      <c r="O13">
+        <v>0.9894885316301043</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>0.9910473724789013</v>
+      </c>
+      <c r="D14">
+        <v>0.9951476542302997</v>
+      </c>
+      <c r="E14">
+        <v>0.9948155183826323</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>0.9905052367312093</v>
+      </c>
+      <c r="H14">
+        <v>0.9960512888049539</v>
+      </c>
+      <c r="J14">
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="L14">
+        <v>0.9867338485001819</v>
+      </c>
+      <c r="M14">
+        <v>0.9946259531284898</v>
+      </c>
+      <c r="N14">
+        <v>0.9905391020553729</v>
+      </c>
+      <c r="O14">
+        <v>0.9891519136333979</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>0.9910122741661758</v>
+      </c>
+      <c r="D15">
+        <v>0.9953816720402139</v>
+      </c>
+      <c r="E15">
+        <v>0.9958997106843204</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>0.991228815928906</v>
+      </c>
+      <c r="H15">
+        <v>0.9962855191125647</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>0.9882829098628939</v>
+      </c>
+      <c r="M15">
+        <v>0.9949031959108006</v>
+      </c>
+      <c r="N15">
+        <v>0.993198593533112</v>
+      </c>
+      <c r="O15">
+        <v>0.9900080232009912</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0.9898648861266423</v>
+      </c>
+      <c r="D16">
+        <v>0.995418453217066</v>
+      </c>
+      <c r="E16">
+        <v>0.9964109003453668</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>0.9928663990099267</v>
+      </c>
+      <c r="H16">
+        <v>0.9963223336882226</v>
+      </c>
+      <c r="J16">
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="L16">
+        <v>0.9878993229734896</v>
+      </c>
+      <c r="M16">
+        <v>0.9950806251766237</v>
+      </c>
+      <c r="N16">
+        <v>0.9944709492595286</v>
+      </c>
+      <c r="O16">
+        <v>0.9920607474815649</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>0.9892884398954911</v>
+      </c>
+      <c r="D17">
+        <v>0.9953851572537726</v>
+      </c>
+      <c r="E17">
+        <v>0.996485320239295</v>
+      </c>
+      <c r="F17">
+        <v>0.9999999999999998</v>
+      </c>
+      <c r="G17">
+        <v>0.9934998378097286</v>
+      </c>
+      <c r="H17">
+        <v>0.9962890074908392</v>
+      </c>
+      <c r="J17">
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="L17">
+        <v>0.9874660410856098</v>
+      </c>
+      <c r="M17">
+        <v>0.9951054367543352</v>
+      </c>
+      <c r="N17">
+        <v>0.994688630587452</v>
+      </c>
+      <c r="O17">
+        <v>0.9928573187592444</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>0.9940477591681391</v>
+      </c>
+      <c r="D18">
+        <v>0.9947691887379668</v>
+      </c>
+      <c r="E18">
+        <v>0.9960381552244415</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0.9825029202106044</v>
+      </c>
+      <c r="H18">
+        <v>0.9956724796505496</v>
+      </c>
+      <c r="J18">
+        <v>0.9999999999999998</v>
+      </c>
+      <c r="L18">
+        <v>0.9921608821781657</v>
+      </c>
+      <c r="M18">
+        <v>0.9935698323709092</v>
+      </c>
+      <c r="N18">
+        <v>0.9941587177363297</v>
+      </c>
+      <c r="O18">
+        <v>0.9788635525865069</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>0.9929467789631036</v>
+      </c>
+      <c r="D19">
+        <v>0.9906928642665799</v>
+      </c>
+      <c r="E19">
+        <v>0.9921593072185186</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0.9611089559593372</v>
+      </c>
+      <c r="H19">
+        <v>0.9915924537106279</v>
+      </c>
+      <c r="J19">
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="L19">
+        <v>0.9889815787837511</v>
+      </c>
+      <c r="M19">
+        <v>0.987994548666092</v>
+      </c>
+      <c r="N19">
+        <v>0.9881870229875505</v>
+      </c>
+      <c r="O19">
+        <v>0.9514546711419518</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>0.9857287020906186</v>
+      </c>
+      <c r="D20">
+        <v>0.9880009352247359</v>
+      </c>
+      <c r="E20">
+        <v>0.9866423475669851</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0.9593582825552284</v>
+      </c>
+      <c r="H20">
+        <v>0.9888980802876466</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>0.9744540606998332</v>
+      </c>
+      <c r="M20">
+        <v>0.9853821903594211</v>
+      </c>
+      <c r="N20">
+        <v>0.9753947335359675</v>
+      </c>
+      <c r="O20">
+        <v>0.9500463009699752</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>0.9887036047845105</v>
+      </c>
+      <c r="D21">
+        <v>0.9889753876248141</v>
+      </c>
+      <c r="E21">
+        <v>0.9888106941146061</v>
+      </c>
+      <c r="F21">
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="G21">
+        <v>0.9593023735143466</v>
+      </c>
+      <c r="H21">
+        <v>0.9898734175301662</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <v>0.9805567510029491</v>
+      </c>
+      <c r="M21">
+        <v>0.9862699954633181</v>
+      </c>
+      <c r="N21">
+        <v>0.9806660341108467</v>
+      </c>
+      <c r="O21">
+        <v>0.9496131417852303</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22">
+        <v>0.9922265071497063</v>
+      </c>
+      <c r="D22">
+        <v>0.9896294137836643</v>
+      </c>
+      <c r="E22">
+        <v>0.9913736146325236</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>0.9559664842551042</v>
+      </c>
+      <c r="H22">
+        <v>0.9905280375713889</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>0.9880763395477189</v>
+      </c>
+      <c r="M22">
+        <v>0.9865929695426309</v>
+      </c>
+      <c r="N22">
+        <v>0.9872153530177266</v>
+      </c>
+      <c r="O22">
+        <v>0.9447938646892488</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23">
+        <v>0.9941299732920263</v>
+      </c>
+      <c r="D23">
+        <v>0.9904691482753921</v>
+      </c>
+      <c r="E23">
+        <v>0.992959334455772</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>0.957153793920178</v>
+      </c>
+      <c r="H23">
+        <v>0.9913685345762143</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>0.9917270766103421</v>
+      </c>
+      <c r="M23">
+        <v>0.9874610559346365</v>
+      </c>
+      <c r="N23">
+        <v>0.9905505710266135</v>
+      </c>
+      <c r="O23">
+        <v>0.9461128576079337</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24">
+        <v>0.995247532258513</v>
+      </c>
+      <c r="D24">
+        <v>0.9906197926260227</v>
+      </c>
+      <c r="E24">
+        <v>0.9938711278553529</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>0.9556219444886158</v>
+      </c>
+      <c r="H24">
+        <v>0.991519315718047</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>0.9940435336590371</v>
+      </c>
+      <c r="M24">
+        <v>0.9874737522007472</v>
+      </c>
+      <c r="N24">
+        <v>0.9926641372389237</v>
+      </c>
+      <c r="O24">
+        <v>0.9439478778856533</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25">
+        <v>0.9958736075553308</v>
+      </c>
+      <c r="D25">
+        <v>0.9913165407382651</v>
+      </c>
+      <c r="E25">
+        <v>0.9946920874470705</v>
+      </c>
+      <c r="F25">
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="G25">
+        <v>0.9585123290777529</v>
+      </c>
+      <c r="H25">
+        <v>0.9922166965059341</v>
+      </c>
+      <c r="J25">
+        <v>0.9999999999999999</v>
+      </c>
+      <c r="L25">
+        <v>0.9951561264273685</v>
+      </c>
+      <c r="M25">
+        <v>0.9883503458902334</v>
+      </c>
+      <c r="N25">
+        <v>0.9939732705840985</v>
+      </c>
+      <c r="O25">
+        <v>0.9476640323827289</v>
       </c>
     </row>
   </sheetData>

</xml_diff>